<commit_message>
Atualização automática de CASCA.xlsx
</commit_message>
<xml_diff>
--- a/CASCA.xlsx
+++ b/CASCA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{533B0262-6D97-4E50-B5AA-0A2ED044691E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{62326AD4-9207-46DE-9404-6D020BE772F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,20 +23,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="7" r:id="rId8"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1239,7 +1226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1300,30 +1287,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1341,7 +1304,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1380,17 +1343,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1437,7 +1395,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{71805DAF-A0CB-4429-B082-B2128343EE08}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{85A45917-19FC-4A4E-A6E4-CF4F4E0BD9F9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1467,10 +1425,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43381AB2-6684-4F31-865E-CD2B5DD271D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C45D8B60-42E8-4941-BFFE-D6C492B8B6EC}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1508,7 +1466,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDBD57E9-DCF0-4BAA-B5D3-F920A21D8910}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{103B7F8A-333A-4B6A-8B24-68F905AA2C9D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1571,7 +1529,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9473209D-7401-48FD-BB12-87394C4C9A9F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{678AC6D4-2E95-4AFE-B98E-FE97C01F7366}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1590,7 +1548,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64BC7606-7723-323D-D105-4A89D3D36E1F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E03C7FD-9D6C-A043-F267-66EC26D45F78}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1639,7 +1597,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BD77BDE-BB4A-AA0C-8A5D-13379EC58370}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61726770-ED99-8BB5-C9C3-E08A418DB89C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1658,7 +1616,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{107EEBF5-DDAA-50D3-6B21-083FE6F12C41}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2A1901F-77EE-216E-5275-79D0EF08E043}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1689,7 +1647,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4C1FF09-A3D9-F379-3262-6666E014C78C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C96AD2C5-5FE0-7CC0-A457-125F65270C8A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1720,7 +1678,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7075393-CB71-5A2F-ADD4-4BC62A896994}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A09B3E3B-D861-2966-50F2-9F2C9221676F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1763,7 +1721,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F0348B9-50FF-4118-9385-85A654439A2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94E2D950-9DB4-469A-B60F-00674D0245AB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1801,7 +1759,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B3F98AD-193B-4226-AACB-0FA21F4DEFBE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0A50105-EF31-4D24-BFEB-C9D5677D27DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1844,7 +1802,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03CD0D73-369A-4F3D-B70E-C2BAB46C969B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{131128D8-D677-4931-9A7A-C7844A9F3576}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2157,7 +2115,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA35C76-3CC6-4C28-A0AF-419D3A8F7DC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE2A976B-6E4F-4F77-8F63-425C287EA300}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2169,98 +2127,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="41"/>
-    <col min="6" max="6" width="2" style="41" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="41" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="41"/>
+    <col min="1" max="5" width="12.5703125" style="38"/>
+    <col min="6" max="6" width="2" style="38" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="38" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="40"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="40"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="40"/>
+      <c r="F3" s="37"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="40"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="40"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="40"/>
+      <c r="F6" s="37"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="40"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="40"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="40"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="40"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="40"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="40"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="40"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="40"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="40"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="40"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="40"/>
+      <c r="F17" s="37"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="40"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="40"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="40"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="40"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="40"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="40"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="40"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="40"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="40"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="40"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="40"/>
+      <c r="F28" s="37"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="40"/>
+      <c r="F29" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5526,19 +5484,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>273</v>
       </c>
     </row>
@@ -5572,46 +5530,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="17" t="s">
         <v>284</v>
       </c>
     </row>
@@ -5619,7 +5577,7 @@
       <c r="A2" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="19">
         <v>196166</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5631,10 +5589,10 @@
       <c r="E2" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="20">
         <v>35.97</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="20">
         <v>359.7</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -5663,7 +5621,7 @@
       <c r="A3" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="19">
         <v>195706</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5675,10 +5633,10 @@
       <c r="E3" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="20">
         <v>28.93</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="20">
         <v>289.3</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -5707,7 +5665,7 @@
       <c r="A4" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="19">
         <v>195723</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -5719,10 +5677,10 @@
       <c r="E4" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="20">
         <v>28.93</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="20">
         <v>289.3</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -5751,7 +5709,7 @@
       <c r="A5" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="19">
         <v>196170</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -5763,10 +5721,10 @@
       <c r="E5" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="20">
         <v>34.799999999999997</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="20">
         <v>348</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -5795,7 +5753,7 @@
       <c r="A6" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="19">
         <v>196177</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -5807,10 +5765,10 @@
       <c r="E6" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="20">
         <v>13.42</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="20">
         <v>134.19999999999999</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -5839,7 +5797,7 @@
       <c r="A7" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="19">
         <v>196168</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -5851,10 +5809,10 @@
       <c r="E7" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="20">
         <v>44.96</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="20">
         <v>449.6</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -5883,7 +5841,7 @@
       <c r="A8" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="19">
         <v>196189</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -5895,10 +5853,10 @@
       <c r="E8" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="20">
         <v>16.39</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="20">
         <v>163.9</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -5927,7 +5885,7 @@
       <c r="A9" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="19">
         <v>195707</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -5939,10 +5897,10 @@
       <c r="E9" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="20">
         <v>6.68</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="20">
         <v>66.8</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -5971,7 +5929,7 @@
       <c r="A10" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="19">
         <v>196194</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -5983,10 +5941,10 @@
       <c r="E10" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="20">
         <v>6.68</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="20">
         <v>66.8</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -6015,7 +5973,7 @@
       <c r="A11" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="19">
         <v>196176</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -6027,10 +5985,10 @@
       <c r="E11" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="20">
         <v>27.7</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="20">
         <v>277</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -6059,7 +6017,7 @@
       <c r="A12" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="19">
         <v>1748</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -6071,10 +6029,10 @@
       <c r="E12" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="20">
         <v>27.7</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="20">
         <v>277</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -6103,7 +6061,7 @@
       <c r="A13" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="19">
         <v>37593</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -6115,10 +6073,10 @@
       <c r="E13" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="20">
         <v>27.7</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="20">
         <v>277</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -6147,7 +6105,7 @@
       <c r="A14" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="19">
         <v>48476</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -6159,10 +6117,10 @@
       <c r="E14" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="20">
         <v>18.899999999999999</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="20">
         <v>189</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -6191,7 +6149,7 @@
       <c r="A15" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="19">
         <v>48484</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -6203,10 +6161,10 @@
       <c r="E15" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="20">
         <v>18.899999999999999</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="20">
         <v>189</v>
       </c>
       <c r="H15" s="2" t="s">
@@ -6235,7 +6193,7 @@
       <c r="A16" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="19">
         <v>107127</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -6247,10 +6205,10 @@
       <c r="E16" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="20">
         <v>30.8</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="20">
         <v>308</v>
       </c>
       <c r="H16" s="2" t="s">
@@ -6279,7 +6237,7 @@
       <c r="A17" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="19">
         <v>226527</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -6291,10 +6249,10 @@
       <c r="E17" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="20">
         <v>19.77</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="20">
         <v>197.68</v>
       </c>
       <c r="H17" s="2" t="s">
@@ -6323,7 +6281,7 @@
       <c r="A18" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="19">
         <v>276827</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -6335,10 +6293,10 @@
       <c r="E18" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="20">
         <v>24.39</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="20">
         <v>243.89</v>
       </c>
       <c r="H18" s="2" t="s">
@@ -6367,7 +6325,7 @@
       <c r="A19" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="19">
         <v>271572</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -6379,10 +6337,10 @@
       <c r="E19" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="20">
         <v>23.8</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="20">
         <v>238</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -6411,7 +6369,7 @@
       <c r="A20" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="19">
         <v>300581</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -6423,10 +6381,10 @@
       <c r="E20" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="20">
         <v>23.8</v>
       </c>
-      <c r="G20" s="23">
+      <c r="G20" s="20">
         <v>238</v>
       </c>
       <c r="H20" s="2" t="s">
@@ -6455,7 +6413,7 @@
       <c r="A21" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="19">
         <v>302343</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -6467,10 +6425,10 @@
       <c r="E21" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="20">
         <v>23.8</v>
       </c>
-      <c r="G21" s="23">
+      <c r="G21" s="20">
         <v>238</v>
       </c>
       <c r="H21" s="2" t="s">
@@ -6499,7 +6457,7 @@
       <c r="A22" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="19">
         <v>327551</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -6511,10 +6469,10 @@
       <c r="E22" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="20">
         <v>22.48</v>
       </c>
-      <c r="G22" s="23">
+      <c r="G22" s="20">
         <v>224.8</v>
       </c>
       <c r="H22" s="2" t="s">
@@ -6543,7 +6501,7 @@
       <c r="A23" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="19">
         <v>352108</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -6555,10 +6513,10 @@
       <c r="E23" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F23" s="23">
+      <c r="F23" s="20">
         <v>18.8</v>
       </c>
-      <c r="G23" s="23">
+      <c r="G23" s="20">
         <v>188</v>
       </c>
       <c r="H23" s="2" t="s">
@@ -6597,14 +6555,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>330</v>
       </c>
     </row>
@@ -6635,46 +6593,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>331</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>333</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>335</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="23" t="s">
         <v>336</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="23" t="s">
         <v>334</v>
       </c>
     </row>
@@ -6699,54 +6657,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>337</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>338</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>339</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>340</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="25" t="s">
         <v>341</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="26" t="s">
         <v>342</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="26" t="s">
         <v>343</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>344</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>345</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>346</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>347</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="24" t="s">
         <v>348</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>349</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="24" t="s">
         <v>350</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="24" t="s">
         <v>351</v>
       </c>
     </row>
@@ -6757,43 +6716,43 @@
       <c r="B2" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="27">
         <v>45108</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="28">
         <v>2001</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="28" t="s">
         <v>353</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="29">
         <v>4146</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="29">
         <v>555</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="30" t="s">
         <v>355</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="30" t="s">
         <v>355</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="30" t="s">
         <v>355</v>
       </c>
-      <c r="M2" s="34" t="s">
+      <c r="M2" s="31" t="s">
         <v>356</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="31" t="s">
         <v>356</v>
       </c>
     </row>
@@ -6824,25 +6783,24 @@
       <c r="B1" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="32" t="s">
         <v>358</v>
       </c>
-      <c r="E1" s="36">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="33">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2" s="36">
         <v>61</v>
       </c>
-      <c r="F1" s="37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>285</v>
-      </c>
-      <c r="B2" s="39">
-        <v>61</v>
-      </c>
-      <c r="C2" s="37">
+      <c r="C2" s="34">
         <v>4.033857955296918E-3</v>
       </c>
     </row>

</xml_diff>